<commit_message>
feat：update map panel point
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/LandMark_大地图地标表.xlsx
+++ b/dragon-verse/Excels/LandMark_大地图地标表.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t xml:space="preserve">Maptext009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imgSymbol9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maptext010</t>
   </si>
 </sst>
 </file>
@@ -153,32 +159,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -374,117 +384,127 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75390625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="51.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="51.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="35.62"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" s="4" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" s="3" customFormat="true" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" s="4" customFormat="true" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="1" t="s">
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+    <row r="5" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+    <row r="7" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" s="2" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>